<commit_message>
rm optimal clustering, update clusters in Table S2
</commit_message>
<xml_diff>
--- a/tables/output/TableS3-SF-dysreg.xlsx
+++ b/tables/output/TableS3-SF-dysreg.xlsx
@@ -2876,7 +2876,7 @@
         <v>0.0177095494749196</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0389610088448231</v>
+        <v>0.038961008844823</v>
       </c>
     </row>
     <row r="5">
@@ -3120,7 +3120,7 @@
         <v>-0.308777961962955</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0787228444338641</v>
+        <v>0.078722844433864</v>
       </c>
       <c r="E15" t="n">
         <v>-3.92234254470267</v>
@@ -3919,7 +3919,7 @@
         <v>150</v>
       </c>
       <c r="B50" t="n">
-        <v>2248.54625600321</v>
+        <v>2248.5462560032</v>
       </c>
       <c r="C50" t="n">
         <v>0.540216206993242</v>

</xml_diff>

<commit_message>
also adding this to table s2
</commit_message>
<xml_diff>
--- a/tables/output/TableS3-SF-dysreg.xlsx
+++ b/tables/output/TableS3-SF-dysreg.xlsx
@@ -2876,7 +2876,7 @@
         <v>0.0177095494749196</v>
       </c>
       <c r="G4" t="n">
-        <v>0.038961008844823</v>
+        <v>0.0389610088448231</v>
       </c>
     </row>
     <row r="5">
@@ -3120,7 +3120,7 @@
         <v>-0.308777961962955</v>
       </c>
       <c r="D15" t="n">
-        <v>0.078722844433864</v>
+        <v>0.0787228444338641</v>
       </c>
       <c r="E15" t="n">
         <v>-3.92234254470267</v>
@@ -3919,7 +3919,7 @@
         <v>150</v>
       </c>
       <c r="B50" t="n">
-        <v>2248.5462560032</v>
+        <v>2248.54625600321</v>
       </c>
       <c r="C50" t="n">
         <v>0.540216206993242</v>

</xml_diff>